<commit_message>
Product order in performance excel sorted
Mongodb bypass added
</commit_message>
<xml_diff>
--- a/Reactive_10Robots/products.xlsx
+++ b/Reactive_10Robots/products.xlsx
@@ -59,7 +59,7 @@
     <t xml:space="preserve">At workstation 7  </t>
   </si>
   <si>
-    <t>12/30/2023, 14:28:50</t>
+    <t>12/31/2023, 00:23:14</t>
   </si>
   <si>
     <t>Product</t>
@@ -80,16 +80,16 @@
     <t>Idle time</t>
   </si>
   <si>
-    <t>Product 1</t>
-  </si>
-  <si>
-    <t>Product 2</t>
-  </si>
-  <si>
-    <t>Product 3</t>
-  </si>
-  <si>
-    <t>Product 4</t>
+    <t>PV-1_PI-1</t>
+  </si>
+  <si>
+    <t>PV-2_PI-1</t>
+  </si>
+  <si>
+    <t>PV-2_PI-2</t>
+  </si>
+  <si>
+    <t>PV-3_PI-1</t>
   </si>
 </sst>
 </file>
@@ -568,7 +568,7 @@
         <v>21</v>
       </c>
       <c r="B2">
-        <v>1000</v>
+        <v>5000</v>
       </c>
       <c r="C2">
         <v>200</v>
@@ -628,7 +628,7 @@
         <v>24</v>
       </c>
       <c r="B5">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="C5">
         <v>200</v>

</xml_diff>